<commit_message>
Added print option to create a print-pdf
</commit_message>
<xml_diff>
--- a/NotenMaster_template.xlsx
+++ b/NotenMaster_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/robin_woerz_bwedu_de/Documents/Dokumente/Python_projects/NotenMaster/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/robin_woerz_bwedu_de/Documents/Dokumente/Python_projects/NotenMaster/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="13_ncr:1_{2E541D44-1ECF-4AD0-8832-968A3B846A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DA73A18-C9D8-4ED4-859A-6EFBBA8C5190}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{2E541D44-1ECF-4AD0-8832-968A3B846A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9C3762E-C18F-4D94-B9AB-E5AE8B7E0A45}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EFBADC28-27DB-455B-A7A5-6DED1BF906AF}"/>
+    <workbookView xWindow="28680" yWindow="4575" windowWidth="20730" windowHeight="11160" xr2:uid="{EFBADC28-27DB-455B-A7A5-6DED1BF906AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="66">
   <si>
     <t>Piccolo</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>Horn in es</t>
+  </si>
+  <si>
+    <t>Druckanzahl</t>
   </si>
 </sst>
 </file>
@@ -284,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -396,30 +399,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -454,19 +441,28 @@
     <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -482,10 +478,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -792,7 +784,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -800,9 +792,9 @@
     <col min="1" max="1" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="2"/>
+    <col min="4" max="4" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="2" customWidth="1"/>
     <col min="8" max="257" width="11.42578125" style="1"/>
     <col min="258" max="258" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1122,37 +1114,41 @@
     <col min="16136" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="F1" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="16">
         <v>1</v>
       </c>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="24"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1161,15 +1157,18 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>1</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="F3" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1178,28 +1177,34 @@
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>2</v>
       </c>
-      <c r="E4" s="18"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="E4" s="21"/>
+      <c r="F4" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>3</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1208,13 +1213,14 @@
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>5</v>
       </c>
-      <c r="E6" s="18"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="E6" s="21"/>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1223,15 +1229,18 @@
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>6</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="F7" s="24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1240,13 +1249,14 @@
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>7</v>
       </c>
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="E8" s="21"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1255,41 +1265,48 @@
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>8</v>
       </c>
-      <c r="E9" s="18"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="E9" s="21"/>
+      <c r="F9" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="9">
+      <c r="C10" s="4"/>
+      <c r="D10" s="8">
         <v>9</v>
       </c>
-      <c r="E10" s="20"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
+      <c r="E10" s="22"/>
+      <c r="F10" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>4</v>
       </c>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
+      <c r="E11" s="23"/>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1298,13 +1315,14 @@
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>10</v>
       </c>
-      <c r="E12" s="18"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+      <c r="E12" s="21"/>
+      <c r="F12" s="24"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1313,11 +1331,12 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="D13" s="16"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="24"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1326,11 +1345,12 @@
       <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+      <c r="D14" s="16"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="24"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1339,24 +1359,26 @@
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="24"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="20"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="26"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="15" t="s">
         <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1365,11 +1387,12 @@
       <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="18"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="15" t="s">
         <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1378,24 +1401,26 @@
       <c r="C18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="18"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="20"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="26"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="15" t="s">
         <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1404,11 +1429,12 @@
       <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="24"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="15" t="s">
         <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1417,12 +1443,12 @@
       <c r="C21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="3"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="25"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="15" t="s">
         <v>63</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1431,24 +1457,26 @@
       <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="26"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1457,11 +1485,12 @@
       <c r="C24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="18"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="24"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1470,12 +1499,12 @@
       <c r="C25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="3"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="25"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1484,24 +1513,26 @@
       <c r="C26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="18"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="24"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="20"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="26"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="15" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1510,11 +1541,12 @@
       <c r="C28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="18"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="24"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="15" t="s">
         <v>52</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1523,11 +1555,12 @@
       <c r="C29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="18"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="24"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="15" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1536,24 +1569,26 @@
       <c r="C30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="18"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="24"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="20"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="26"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="15" t="s">
         <v>53</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1562,11 +1597,12 @@
       <c r="C32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="18"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
+      <c r="D32" s="16"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="24"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
         <v>53</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1575,11 +1611,12 @@
       <c r="C33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="17"/>
-      <c r="E33" s="18"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="16" t="s">
+      <c r="D33" s="16"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="24"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
         <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1588,24 +1625,26 @@
       <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="18"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="24"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="20"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
+      <c r="D35" s="8"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="26"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1614,11 +1653,12 @@
       <c r="C36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="18"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="16" t="s">
+      <c r="D36" s="16"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="24"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1627,24 +1667,26 @@
       <c r="C37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="18"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="19" t="s">
+      <c r="D37" s="16"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="24"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="20"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="16" t="s">
+      <c r="D38" s="8"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="26"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1653,24 +1695,26 @@
       <c r="C39" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="17"/>
-      <c r="E39" s="18"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="19" t="s">
+      <c r="D39" s="16"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="24"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="20"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
+      <c r="D40" s="8"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="26"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1679,11 +1723,12 @@
       <c r="C41" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="18"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="16" t="s">
+      <c r="D41" s="16"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="24"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1692,11 +1737,12 @@
       <c r="C42" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="18"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="16" t="s">
+      <c r="D42" s="16"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="24"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1705,64 +1751,70 @@
       <c r="C43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="18"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="19" t="s">
+      <c r="D43" s="16"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="24"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="20"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="21" t="s">
+      <c r="D44" s="8"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="26"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="22"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="16" t="s">
+      <c r="C45" s="6"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="26"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="18"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="19" t="s">
+      <c r="D46" s="16"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="24"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="20"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="19" t="s">
+      <c r="C47" s="4"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="26"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="20"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="26"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>

</xml_diff>